<commit_message>
Added Note column in iic_addresses.xlsx
</commit_message>
<xml_diff>
--- a/peripherals/iic_addresses.xlsx
+++ b/peripherals/iic_addresses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ismael\Dropbox\GAPS\DRS4_V2\I2C_Address\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/takeruhayashi/GAPS/drs4-board/peripherals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C8C28A-8F0A-4A44-80EA-AAB92CE0AB0D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F5AF5DB-C86B-C741-B4F4-9932A6502E26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42975" yWindow="2955" windowWidth="21600" windowHeight="11385" xr2:uid="{2BA2EAEC-3DFF-4586-94A5-FF23E16BC420}"/>
+    <workbookView xWindow="-49820" yWindow="3940" windowWidth="26480" windowHeight="19080" xr2:uid="{2BA2EAEC-3DFF-4586-94A5-FF23E16BC420}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Sheet</t>
   </si>
@@ -84,6 +78,12 @@
     <t>0x42
 0x43
 0x44</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>DRS4 Temperature Sensor</t>
   </si>
 </sst>
 </file>
@@ -466,20 +466,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56C3EC7B-C017-4BEB-ADB0-84AE6F56AD33}">
-  <dimension ref="A2:C11"/>
+  <dimension ref="A2:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="3" max="4" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -489,8 +489,11 @@
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>11</v>
       </c>
@@ -500,8 +503,9 @@
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="3" t="s">
         <v>7</v>
@@ -509,8 +513,9 @@
       <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>13</v>
       </c>
@@ -520,8 +525,9 @@
       <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>15</v>
       </c>
@@ -531,8 +537,9 @@
       <c r="C6" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>18</v>
       </c>
@@ -542,8 +549,9 @@
       <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
         <v>7</v>
@@ -551,8 +559,11 @@
       <c r="C8" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D8" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>19</v>
       </c>
@@ -562,8 +573,9 @@
       <c r="C9" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
         <v>7</v>
@@ -571,8 +583,9 @@
       <c r="C10" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>23</v>
       </c>
@@ -582,6 +595,7 @@
       <c r="C11" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="D11" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>